<commit_message>
Updated OutlookLogin and OpenAir
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData-1.xlsx
+++ b/src/test/resources/testdata/TestData-1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14850" windowHeight="6020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14850" windowHeight="6020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="51">
   <si>
     <t>TC_ID</t>
   </si>
@@ -160,6 +160,30 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>lifecycle</t>
+  </si>
+  <si>
+    <t>depends_TC</t>
+  </si>
+  <si>
+    <t>outlookLogin</t>
+  </si>
+  <si>
+    <t>http://mail.maveric-systems.com/</t>
+  </si>
+  <si>
+    <t>driverType</t>
+  </si>
+  <si>
+    <t>desktop</t>
+  </si>
+  <si>
+    <t>danielf@maveric-systems.com</t>
+  </si>
+  <si>
+    <t>Mavaug@123</t>
   </si>
 </sst>
 </file>
@@ -523,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,6 +854,9 @@
       <c r="L8" s="1" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G15" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -949,12 +976,98 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>